<commit_message>
Change name Face Detection
</commit_message>
<xml_diff>
--- a/Document/Tasksheet.xlsx
+++ b/Document/Tasksheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="40" documentId="11_F25DC773A252ABEACE02EC619BD849EA5BDE5894" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{BC60421C-C6EA-415F-8569-10E81AD20178}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0580BF4F-9F86-44BA-A9BF-7FD31F5F6188}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="22308" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -557,10 +557,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t xml:space="preserve">                &lt;Server&gt; Face Analysis</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t xml:space="preserve">                &lt;Server&gt; Connect to web</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -574,6 +570,10 @@
   </si>
   <si>
     <t xml:space="preserve">        User Interface Design</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t xml:space="preserve">                &lt;Server&gt; Face Detection</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -1053,8 +1053,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H179"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="D165" sqref="D165"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="B108" sqref="B108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
@@ -1836,7 +1836,7 @@
     <row r="62" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A62" s="13"/>
       <c r="B62" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C62" s="5" t="s">
         <v>70</v>
@@ -2368,7 +2368,7 @@
     <row r="105" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A105" s="13"/>
       <c r="B105" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C105" s="5" t="s">
         <v>70</v>
@@ -2396,7 +2396,7 @@
     <row r="107" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A107" s="13"/>
       <c r="B107" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C107" s="5"/>
       <c r="D107" s="5" t="s">
@@ -2410,7 +2410,7 @@
     <row r="108" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A108" s="13"/>
       <c r="B108" s="4" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="C108" s="5"/>
       <c r="D108" s="5"/>
@@ -2448,7 +2448,7 @@
     <row r="111" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A111" s="13"/>
       <c r="B111" s="7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C111" s="5"/>
       <c r="D111" s="5"/>

</xml_diff>